<commit_message>
Enhance garments data window with dynamic table and progress bars for fabric status
</commit_message>
<xml_diff>
--- a/garments_status_output.xlsx
+++ b/garments_status_output.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,17 +466,17 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Order Qty (Pcs)</t>
+          <t>Order Qty</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Cutting Qty (Pcs)</t>
+          <t>Cutting Qty</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Cutting Rejection (Pcs)</t>
+          <t>Cutting Rejection</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
@@ -486,92 +486,106 @@
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Input Qty (Pcs)</t>
+          <t>Input Qty</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Sewing Rejection (Pcs)</t>
+          <t>Sewing Rejection</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>Output Qty (Pcs)</t>
+          <t>Output Qty</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>Finishing Rejection (Pcs)</t>
+          <t>Finishing Rejection</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>Poly Qty (Pcs)</t>
+          <t>Poly Qty</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>Leftover/Rej Qty (Pcs)</t>
+          <t>Leftover/Rej Qty</t>
         </is>
       </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>Floor Shipped Qty (Pcs)</t>
+          <t>Floor Shipped Qty</t>
         </is>
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>Ex-Factory Shipped Qty (Pcs)</t>
-        </is>
-      </c>
-      <c r="O1" s="2" t="inlineStr">
-        <is>
-          <t>Prod Floor</t>
+          <t>Ex-Factory Shipped Qty</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>2025/12649</t>
+          <t>2025/13874</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>CAMEL ACTIVE</t>
+          <t>G-STAR</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D2" s="3" t="inlineStr"/>
-      <c r="E2" s="3" t="inlineStr"/>
-      <c r="F2" s="3" t="inlineStr"/>
-      <c r="G2" s="3" t="inlineStr"/>
-      <c r="H2" s="3" t="inlineStr"/>
-      <c r="I2" s="3" t="inlineStr"/>
-      <c r="J2" s="3" t="inlineStr"/>
-      <c r="K2" s="3" t="inlineStr"/>
-      <c r="L2" s="3" t="inlineStr"/>
+        <v>4000</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>6367</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>2999</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>2866</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>1110</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="M2" s="3" t="inlineStr"/>
       <c r="N2" s="3" t="inlineStr"/>
-      <c r="O2" s="3" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>2025/11734</t>
+          <t>2025/12862</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>CAMEL ACTIVE</t>
+          <t>G-STAR</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D3" s="3" t="inlineStr"/>
+        <v>19212</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>4223</v>
+      </c>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="3" t="inlineStr"/>
@@ -582,23 +596,24 @@
       <c r="L3" s="3" t="inlineStr"/>
       <c r="M3" s="3" t="inlineStr"/>
       <c r="N3" s="3" t="inlineStr"/>
-      <c r="O3" s="3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>2025/11999</t>
+          <t>2025/12987</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>CAMEL ACTIVE</t>
+          <t>G-STAR</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>4500</v>
-      </c>
-      <c r="D4" s="3" t="inlineStr"/>
+        <v>2926</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>210</v>
+      </c>
       <c r="E4" s="3" t="inlineStr"/>
       <c r="F4" s="3" t="inlineStr"/>
       <c r="G4" s="3" t="inlineStr"/>
@@ -609,34 +624,224 @@
       <c r="L4" s="3" t="inlineStr"/>
       <c r="M4" s="3" t="inlineStr"/>
       <c r="N4" s="3" t="inlineStr"/>
-      <c r="O4" s="3" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>2025/11988</t>
+          <t>2025/13860</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>CAMEL ACTIVE</t>
+          <t>G-STAR</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>2500</v>
-      </c>
-      <c r="D5" s="3" t="inlineStr"/>
-      <c r="E5" s="3" t="inlineStr"/>
-      <c r="F5" s="3" t="inlineStr"/>
-      <c r="G5" s="3" t="inlineStr"/>
-      <c r="H5" s="3" t="inlineStr"/>
-      <c r="I5" s="3" t="inlineStr"/>
-      <c r="J5" s="3" t="inlineStr"/>
+        <v>1200</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>1248</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>1246</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>1246</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>9</v>
+      </c>
       <c r="K5" s="3" t="inlineStr"/>
-      <c r="L5" s="3" t="inlineStr"/>
+      <c r="L5" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="M5" s="3" t="inlineStr"/>
       <c r="N5" s="3" t="inlineStr"/>
-      <c r="O5" s="3" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>2025/12898</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>G-STAR</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>38475</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>3451</v>
+      </c>
+      <c r="E6" s="3" t="inlineStr"/>
+      <c r="F6" s="3" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
+      <c r="I6" s="3" t="inlineStr"/>
+      <c r="J6" s="3" t="inlineStr"/>
+      <c r="K6" s="3" t="inlineStr"/>
+      <c r="L6" s="3" t="inlineStr"/>
+      <c r="M6" s="3" t="inlineStr"/>
+      <c r="N6" s="3" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>2025/12878</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>G-STAR</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>6369</v>
+      </c>
+      <c r="D7" s="3" t="inlineStr"/>
+      <c r="E7" s="3" t="inlineStr"/>
+      <c r="F7" s="3" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr"/>
+      <c r="I7" s="3" t="inlineStr"/>
+      <c r="J7" s="3" t="inlineStr"/>
+      <c r="K7" s="3" t="inlineStr"/>
+      <c r="L7" s="3" t="inlineStr"/>
+      <c r="M7" s="3" t="inlineStr"/>
+      <c r="N7" s="3" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>2025/13762</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>G-STAR</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D8" s="3" t="inlineStr"/>
+      <c r="E8" s="3" t="inlineStr"/>
+      <c r="F8" s="3" t="inlineStr"/>
+      <c r="G8" s="3" t="inlineStr"/>
+      <c r="H8" s="3" t="inlineStr"/>
+      <c r="I8" s="3" t="inlineStr"/>
+      <c r="J8" s="3" t="inlineStr"/>
+      <c r="K8" s="3" t="inlineStr"/>
+      <c r="L8" s="3" t="inlineStr"/>
+      <c r="M8" s="3" t="inlineStr"/>
+      <c r="N8" s="3" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>2025/12827</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>G-STAR</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>29092</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="E9" s="3" t="inlineStr"/>
+      <c r="F9" s="3" t="inlineStr"/>
+      <c r="G9" s="3" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr"/>
+      <c r="I9" s="3" t="inlineStr"/>
+      <c r="J9" s="3" t="inlineStr"/>
+      <c r="K9" s="3" t="inlineStr"/>
+      <c r="L9" s="3" t="inlineStr"/>
+      <c r="M9" s="3" t="inlineStr"/>
+      <c r="N9" s="3" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>2025/13868</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>G-STAR</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>8963</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>6602</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>4657</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="inlineStr"/>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3" t="inlineStr"/>
+      <c r="N10" s="3" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>2025/13093</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>G-STAR</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>20182</v>
+      </c>
+      <c r="D11" s="3" t="inlineStr"/>
+      <c r="E11" s="3" t="inlineStr"/>
+      <c r="F11" s="3" t="inlineStr"/>
+      <c r="G11" s="3" t="inlineStr"/>
+      <c r="H11" s="3" t="inlineStr"/>
+      <c r="I11" s="3" t="inlineStr"/>
+      <c r="J11" s="3" t="inlineStr"/>
+      <c r="K11" s="3" t="inlineStr"/>
+      <c r="L11" s="3" t="inlineStr"/>
+      <c r="M11" s="3" t="inlineStr"/>
+      <c r="N11" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>